<commit_message>
bunch of excel and examples of retrieval
</commit_message>
<xml_diff>
--- a/data/data_availability.xlsx
+++ b/data/data_availability.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="586">
   <si>
     <t>Fiscal</t>
   </si>
@@ -1676,6 +1676,122 @@
   </si>
   <si>
     <t>operaciones_gobierno_general_all_years_all_alc_cepalstat.xlsx</t>
+  </si>
+  <si>
+    <t>ingresos  sector publico no financiero</t>
+  </si>
+  <si>
+    <t>ingresos tributarios  sector publico no financiero</t>
+  </si>
+  <si>
+    <t>ingresos no tributarios  sector publico no financiero</t>
+  </si>
+  <si>
+    <t>gastos  sector publico no financiero</t>
+  </si>
+  <si>
+    <t>gastos de capital sector publico no financiero</t>
+  </si>
+  <si>
+    <t>gasto adquision activo fijo  sector publico no financiero</t>
+  </si>
+  <si>
+    <t>gasto transferencias de capital  sector publico no financiero</t>
+  </si>
+  <si>
+    <t>gasto intereses sector publico no financiero</t>
+  </si>
+  <si>
+    <t>resultado final sector publico no financiero</t>
+  </si>
+  <si>
+    <t>1990-2015</t>
+  </si>
+  <si>
+    <t>operaciones_spnf_central_all_years_alc_cepalstat.xlsx</t>
+  </si>
+  <si>
+    <t>financiamiento total</t>
+  </si>
+  <si>
+    <t>financiamiento externo</t>
+  </si>
+  <si>
+    <t>financiamiento interno</t>
+  </si>
+  <si>
+    <t>financiamiento otro</t>
+  </si>
+  <si>
+    <t>1990-2012</t>
+  </si>
+  <si>
+    <t>1990-2012: COL, CRI, SLV, GTM, HTI, HND, PRY, PAR, VEN
+1991-2012: NIC
+1990-1998: URY
+1995-2012: DOM</t>
+  </si>
+  <si>
+    <t>1990-2012: CHL, COL, CRI, SLV, GTM, HTI, HND, PRY, PAR, VEN
+1991-2012: NIC
+1995-2012: DOM</t>
+  </si>
+  <si>
+    <t>1990-2012: BOL, CHL, CRI, NIC, PER
+2001-2008: URY</t>
+  </si>
+  <si>
+    <t>financiamiento total gobierno general</t>
+  </si>
+  <si>
+    <t>financiamiento interno gobierno general</t>
+  </si>
+  <si>
+    <t>financiamiento externo gobierno general</t>
+  </si>
+  <si>
+    <t>financiamiento otro gobierno general</t>
+  </si>
+  <si>
+    <t>1990-2012: BOL, CRI, NIC, PER
+2001-2008: URY</t>
+  </si>
+  <si>
+    <t>financiamiento total sector publico no financiero</t>
+  </si>
+  <si>
+    <t>financiamiento interno sector publico no financiero</t>
+  </si>
+  <si>
+    <t>financiamiento externo sector publico no financiero</t>
+  </si>
+  <si>
+    <t>financiamiento otro sector publico no financiero</t>
+  </si>
+  <si>
+    <t>1990-2012: BOL, SLV, MEX, PER
+1990-2011: VEN
+1990-2010: CRI, PRY
+1991-2012: NIC
+1995-2012: ECU
+1990-2007: COL</t>
+  </si>
+  <si>
+    <t>1990-2012: BOL, SLV, MEX, PER
+1990-2011: VEN
+1990-2010: CRI, PRY
+1991-2012: NIC
+1995-2012: ECU
+1998-2004: COL</t>
+  </si>
+  <si>
+    <t>financiamiento_spnf_central_all_years_all_alc_cepalstat.xlsx</t>
+  </si>
+  <si>
+    <t>financiamiento_gobierno_general_all_years_all_alc_cepalstat.xlsx</t>
+  </si>
+  <si>
+    <t>financiamiento_gobierno_central_all_years_all_alc_cepalstat.xlsx</t>
   </si>
 </sst>
 </file>
@@ -2128,10 +2244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R271"/>
+  <dimension ref="A1:R286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2139,8 +2255,8 @@
     <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
     <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27.5703125" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
@@ -2290,21 +2406,21 @@
         <v>423</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="30.75" thickBot="1">
+    <row r="9" spans="1:18" ht="75.75" thickBot="1">
       <c r="B9" t="s">
-        <v>12</v>
+        <v>564</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>354</v>
+      <c r="D9" t="s">
+        <v>568</v>
       </c>
       <c r="E9" t="s">
         <v>355</v>
       </c>
-      <c r="F9" t="s">
-        <v>362</v>
+      <c r="F9" s="2" t="s">
+        <v>570</v>
       </c>
       <c r="G9" t="s">
         <v>356</v>
@@ -2316,43 +2432,27 @@
         <v>359</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>360</v>
+        <v>585</v>
       </c>
       <c r="K9" t="s">
         <v>361</v>
       </c>
-      <c r="N9" s="12" t="s">
-        <v>424</v>
-      </c>
-      <c r="O9" s="13">
-        <v>44</v>
-      </c>
-      <c r="P9" s="13" t="s">
-        <v>425</v>
-      </c>
-      <c r="Q9" s="13" t="s">
-        <v>426</v>
-      </c>
-      <c r="R9" s="13" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="30.75" thickBot="1">
+      <c r="N9" s="12"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" thickBot="1">
       <c r="B10" t="s">
-        <v>348</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>354</v>
+        <v>566</v>
+      </c>
+      <c r="D10" t="s">
+        <v>568</v>
       </c>
       <c r="E10" t="s">
         <v>355</v>
       </c>
-      <c r="F10" t="s">
-        <v>362</v>
-      </c>
       <c r="G10" t="s">
         <v>356</v>
       </c>
@@ -2363,42 +2463,29 @@
         <v>359</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>360</v>
+        <v>585</v>
       </c>
       <c r="K10" t="s">
         <v>361</v>
       </c>
-      <c r="N10" s="12" t="s">
-        <v>428</v>
-      </c>
-      <c r="O10" s="13">
-        <v>52</v>
-      </c>
-      <c r="P10" s="13" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q10" s="13" t="s">
-        <v>430</v>
-      </c>
-      <c r="R10" s="13" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="51.75" thickBot="1">
+      <c r="N10" s="12"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+    </row>
+    <row r="11" spans="1:18" ht="90.75" thickBot="1">
       <c r="B11" t="s">
-        <v>349</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>354</v>
+        <v>565</v>
+      </c>
+      <c r="D11" t="s">
+        <v>568</v>
       </c>
       <c r="E11" t="s">
         <v>355</v>
       </c>
-      <c r="F11" t="s">
-        <v>362</v>
+      <c r="F11" s="2" t="s">
+        <v>569</v>
       </c>
       <c r="G11" t="s">
         <v>356</v>
@@ -2410,41 +2497,27 @@
         <v>359</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>360</v>
+        <v>585</v>
       </c>
       <c r="K11" t="s">
         <v>361</v>
       </c>
-      <c r="N11" s="12" t="s">
-        <v>431</v>
-      </c>
-      <c r="O11" s="13">
-        <v>535</v>
-      </c>
-      <c r="P11" s="13" t="s">
-        <v>432</v>
-      </c>
-      <c r="Q11" s="13" t="s">
-        <v>433</v>
-      </c>
+      <c r="N11" s="12"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
       <c r="R11" s="13"/>
     </row>
-    <row r="12" spans="1:18" ht="39" thickBot="1">
+    <row r="12" spans="1:18" ht="15.75" thickBot="1">
       <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>354</v>
+        <v>567</v>
+      </c>
+      <c r="D12" t="s">
+        <v>568</v>
       </c>
       <c r="E12" t="s">
         <v>355</v>
       </c>
-      <c r="F12" t="s">
-        <v>362</v>
-      </c>
       <c r="G12" t="s">
         <v>356</v>
       </c>
@@ -2455,30 +2528,20 @@
         <v>359</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>360</v>
+        <v>585</v>
       </c>
       <c r="K12" t="s">
         <v>361</v>
       </c>
-      <c r="N12" s="12" t="s">
-        <v>434</v>
-      </c>
-      <c r="O12" s="13">
-        <v>92</v>
-      </c>
-      <c r="P12" s="13" t="s">
-        <v>435</v>
-      </c>
-      <c r="Q12" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="R12" s="13" t="s">
-        <v>437</v>
-      </c>
+      <c r="N12" s="12"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
     </row>
     <row r="13" spans="1:18" ht="30.75" thickBot="1">
       <c r="B13" t="s">
-        <v>350</v>
+        <v>12</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2508,24 +2571,24 @@
         <v>361</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="O13" s="13">
-        <v>136</v>
+        <v>44</v>
       </c>
       <c r="P13" s="13" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
       <c r="Q13" s="13" t="s">
-        <v>440</v>
+        <v>426</v>
       </c>
       <c r="R13" s="13" t="s">
-        <v>441</v>
+        <v>427</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="30.75" thickBot="1">
       <c r="B14" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2555,24 +2618,24 @@
         <v>361</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>442</v>
+        <v>428</v>
       </c>
       <c r="O14" s="13">
-        <v>192</v>
+        <v>52</v>
       </c>
       <c r="P14" s="13" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
       <c r="Q14" s="13" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
       <c r="R14" s="13" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="30.75" thickBot="1">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="51.75" thickBot="1">
       <c r="B15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -2602,22 +2665,22 @@
         <v>361</v>
       </c>
       <c r="N15" s="12" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
       <c r="O15" s="13">
-        <v>531</v>
+        <v>535</v>
       </c>
       <c r="P15" s="13" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
       <c r="Q15" s="13" t="s">
-        <v>447</v>
+        <v>433</v>
       </c>
       <c r="R15" s="13"/>
     </row>
-    <row r="16" spans="1:18" ht="30.75" thickBot="1">
+    <row r="16" spans="1:18" ht="39" thickBot="1">
       <c r="B16" t="s">
-        <v>353</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2647,24 +2710,24 @@
         <v>361</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>448</v>
+        <v>434</v>
       </c>
       <c r="O16" s="13">
-        <v>212</v>
+        <v>92</v>
       </c>
       <c r="P16" s="13" t="s">
-        <v>449</v>
+        <v>435</v>
       </c>
       <c r="Q16" s="13" t="s">
-        <v>450</v>
+        <v>436</v>
       </c>
       <c r="R16" s="13" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="17" spans="2:18" ht="39" thickBot="1">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" ht="30.75" thickBot="1">
       <c r="B17" t="s">
-        <v>27</v>
+        <v>350</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2694,24 +2757,24 @@
         <v>361</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>452</v>
+        <v>438</v>
       </c>
       <c r="O17" s="13">
-        <v>214</v>
+        <v>136</v>
       </c>
       <c r="P17" s="13" t="s">
-        <v>451</v>
+        <v>439</v>
       </c>
       <c r="Q17" s="13" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="R17" s="13" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
     </row>
     <row r="18" spans="2:18" ht="30.75" thickBot="1">
       <c r="B18" t="s">
-        <v>28</v>
+        <v>352</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2741,319 +2804,331 @@
         <v>361</v>
       </c>
       <c r="N18" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="O18" s="13">
+        <v>192</v>
+      </c>
+      <c r="P18" s="13" t="s">
+        <v>443</v>
+      </c>
+      <c r="Q18" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="R18" s="13" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" ht="30.75" thickBot="1">
+      <c r="B19" t="s">
+        <v>351</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E19" t="s">
+        <v>355</v>
+      </c>
+      <c r="F19" t="s">
+        <v>362</v>
+      </c>
+      <c r="G19" t="s">
+        <v>356</v>
+      </c>
+      <c r="H19" t="s">
+        <v>358</v>
+      </c>
+      <c r="I19" t="s">
+        <v>359</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="K19" t="s">
+        <v>361</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>445</v>
+      </c>
+      <c r="O19" s="13">
+        <v>531</v>
+      </c>
+      <c r="P19" s="13" t="s">
+        <v>446</v>
+      </c>
+      <c r="Q19" s="13" t="s">
+        <v>447</v>
+      </c>
+      <c r="R19" s="13"/>
+    </row>
+    <row r="20" spans="2:18" ht="30.75" thickBot="1">
+      <c r="B20" t="s">
+        <v>353</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E20" t="s">
+        <v>355</v>
+      </c>
+      <c r="F20" t="s">
+        <v>362</v>
+      </c>
+      <c r="G20" t="s">
+        <v>356</v>
+      </c>
+      <c r="H20" t="s">
+        <v>358</v>
+      </c>
+      <c r="I20" t="s">
+        <v>359</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="K20" t="s">
+        <v>361</v>
+      </c>
+      <c r="N20" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="O20" s="13">
+        <v>212</v>
+      </c>
+      <c r="P20" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="Q20" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="R20" s="13" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" ht="39" thickBot="1">
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E21" t="s">
+        <v>355</v>
+      </c>
+      <c r="F21" t="s">
+        <v>362</v>
+      </c>
+      <c r="G21" t="s">
+        <v>356</v>
+      </c>
+      <c r="H21" t="s">
+        <v>358</v>
+      </c>
+      <c r="I21" t="s">
+        <v>359</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="K21" t="s">
+        <v>361</v>
+      </c>
+      <c r="N21" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="O21" s="13">
+        <v>214</v>
+      </c>
+      <c r="P21" s="13" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q21" s="13" t="s">
+        <v>453</v>
+      </c>
+      <c r="R21" s="13" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" ht="30.75" thickBot="1">
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E22" t="s">
+        <v>355</v>
+      </c>
+      <c r="F22" t="s">
+        <v>362</v>
+      </c>
+      <c r="G22" t="s">
+        <v>356</v>
+      </c>
+      <c r="H22" t="s">
+        <v>358</v>
+      </c>
+      <c r="I22" t="s">
+        <v>359</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="K22" t="s">
+        <v>361</v>
+      </c>
+      <c r="N22" s="12" t="s">
         <v>455</v>
       </c>
-      <c r="O18" s="13">
+      <c r="O22" s="13">
         <v>308</v>
       </c>
-      <c r="P18" s="13" t="s">
+      <c r="P22" s="13" t="s">
         <v>456</v>
       </c>
-      <c r="Q18" s="13" t="s">
+      <c r="Q22" s="13" t="s">
         <v>457</v>
       </c>
-      <c r="R18" s="13" t="s">
+      <c r="R22" s="13" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="19" spans="2:18" ht="26.25" thickBot="1">
-      <c r="N19" s="12" t="s">
+    <row r="23" spans="2:18" ht="26.25" thickBot="1">
+      <c r="N23" s="12" t="s">
         <v>459</v>
       </c>
-      <c r="O19" s="13">
+      <c r="O23" s="13">
         <v>312</v>
       </c>
-      <c r="P19" s="13" t="s">
+      <c r="P23" s="13" t="s">
         <v>460</v>
       </c>
-      <c r="Q19" s="13" t="s">
+      <c r="Q23" s="13" t="s">
         <v>461</v>
       </c>
-      <c r="R19" s="13" t="s">
+      <c r="R23" s="13" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="20" spans="2:18" ht="15.75" thickBot="1">
-      <c r="B20" t="s">
+    <row r="24" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B24" t="s">
         <v>14</v>
-      </c>
-      <c r="N20" s="12" t="s">
-        <v>462</v>
-      </c>
-      <c r="O20" s="13">
-        <v>332</v>
-      </c>
-      <c r="P20" s="13" t="s">
-        <v>463</v>
-      </c>
-      <c r="Q20" s="13" t="s">
-        <v>464</v>
-      </c>
-      <c r="R20" s="13" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="21" spans="2:18" ht="15.75" thickBot="1">
-      <c r="B21" t="s">
-        <v>15</v>
-      </c>
-      <c r="N21" s="12" t="s">
-        <v>466</v>
-      </c>
-      <c r="O21" s="13">
-        <v>388</v>
-      </c>
-      <c r="P21" s="13" t="s">
-        <v>467</v>
-      </c>
-      <c r="Q21" s="13" t="s">
-        <v>468</v>
-      </c>
-      <c r="R21" s="13" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="22" spans="2:18" ht="26.25" thickBot="1">
-      <c r="B22" t="s">
-        <v>16</v>
-      </c>
-      <c r="N22" s="12" t="s">
-        <v>469</v>
-      </c>
-      <c r="O22" s="13">
-        <v>474</v>
-      </c>
-      <c r="P22" s="13" t="s">
-        <v>470</v>
-      </c>
-      <c r="Q22" s="13" t="s">
-        <v>471</v>
-      </c>
-      <c r="R22" s="13" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="23" spans="2:18" ht="26.25" thickBot="1">
-      <c r="B23" t="s">
-        <v>17</v>
-      </c>
-      <c r="N23" s="12" t="s">
-        <v>473</v>
-      </c>
-      <c r="O23" s="13">
-        <v>500</v>
-      </c>
-      <c r="P23" s="13" t="s">
-        <v>474</v>
-      </c>
-      <c r="Q23" s="13" t="s">
-        <v>475</v>
-      </c>
-      <c r="R23" s="13" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="24" spans="2:18" ht="26.25" thickBot="1">
-      <c r="B24" t="s">
-        <v>18</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
-      <c r="D24" t="s">
-        <v>369</v>
-      </c>
-      <c r="E24" t="s">
-        <v>355</v>
-      </c>
-      <c r="F24" t="s">
-        <v>551</v>
-      </c>
-      <c r="G24" t="s">
-        <v>356</v>
-      </c>
-      <c r="H24" t="s">
-        <v>358</v>
-      </c>
-      <c r="I24" t="s">
-        <v>359</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="K24" t="s">
-        <v>361</v>
-      </c>
       <c r="N24" s="12" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
       <c r="O24" s="13">
-        <v>630</v>
+        <v>332</v>
       </c>
       <c r="P24" s="13" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="Q24" s="13" t="s">
-        <v>479</v>
+        <v>464</v>
       </c>
       <c r="R24" s="13" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="25" spans="2:18" ht="39" thickBot="1">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" ht="15.75" thickBot="1">
       <c r="B25" t="s">
-        <v>363</v>
+        <v>15</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="D25" t="s">
-        <v>369</v>
-      </c>
-      <c r="E25" t="s">
-        <v>355</v>
-      </c>
-      <c r="F25" t="s">
-        <v>551</v>
-      </c>
-      <c r="G25" t="s">
-        <v>356</v>
-      </c>
-      <c r="H25" t="s">
-        <v>358</v>
-      </c>
-      <c r="I25" t="s">
-        <v>359</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="K25" t="s">
-        <v>361</v>
-      </c>
       <c r="N25" s="12" t="s">
-        <v>481</v>
+        <v>466</v>
       </c>
       <c r="O25" s="13">
-        <v>652</v>
+        <v>388</v>
       </c>
       <c r="P25" s="13" t="s">
-        <v>482</v>
+        <v>467</v>
       </c>
       <c r="Q25" s="13" t="s">
-        <v>483</v>
-      </c>
-      <c r="R25" s="13"/>
+        <v>468</v>
+      </c>
+      <c r="R25" s="13" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="26" spans="2:18" ht="26.25" thickBot="1">
       <c r="B26" t="s">
-        <v>364</v>
+        <v>16</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" t="s">
-        <v>369</v>
-      </c>
-      <c r="E26" t="s">
-        <v>355</v>
-      </c>
-      <c r="F26" t="s">
-        <v>551</v>
-      </c>
-      <c r="G26" t="s">
-        <v>356</v>
-      </c>
-      <c r="H26" t="s">
-        <v>358</v>
-      </c>
-      <c r="I26" t="s">
-        <v>359</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="K26" t="s">
-        <v>361</v>
-      </c>
       <c r="N26" s="12" t="s">
-        <v>484</v>
+        <v>469</v>
       </c>
       <c r="O26" s="13">
-        <v>659</v>
+        <v>474</v>
       </c>
       <c r="P26" s="13" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="Q26" s="13" t="s">
-        <v>486</v>
+        <v>471</v>
       </c>
       <c r="R26" s="13" t="s">
-        <v>487</v>
+        <v>472</v>
       </c>
     </row>
     <row r="27" spans="2:18" ht="26.25" thickBot="1">
       <c r="B27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
-      <c r="D27" t="s">
-        <v>369</v>
-      </c>
-      <c r="E27" t="s">
-        <v>355</v>
-      </c>
-      <c r="F27" t="s">
-        <v>551</v>
-      </c>
-      <c r="G27" t="s">
-        <v>356</v>
-      </c>
-      <c r="H27" t="s">
-        <v>358</v>
-      </c>
-      <c r="I27" t="s">
-        <v>359</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="K27" t="s">
-        <v>361</v>
-      </c>
       <c r="N27" s="12" t="s">
-        <v>488</v>
+        <v>473</v>
       </c>
       <c r="O27" s="13">
-        <v>662</v>
+        <v>500</v>
       </c>
       <c r="P27" s="13" t="s">
-        <v>489</v>
+        <v>474</v>
       </c>
       <c r="Q27" s="13" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
       <c r="R27" s="13" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="28" spans="2:18" ht="26.25" thickBot="1">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" ht="45.75" thickBot="1">
       <c r="B28" t="s">
-        <v>365</v>
+        <v>572</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>369</v>
+        <v>568</v>
       </c>
       <c r="E28" t="s">
         <v>355</v>
       </c>
-      <c r="F28" t="s">
-        <v>551</v>
+      <c r="F28" s="2" t="s">
+        <v>571</v>
       </c>
       <c r="G28" t="s">
         <v>356</v>
@@ -3065,43 +3140,27 @@
         <v>359</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="K28" t="s">
-        <v>361</v>
-      </c>
-      <c r="N28" s="12" t="s">
-        <v>492</v>
-      </c>
-      <c r="O28" s="13">
-        <v>663</v>
-      </c>
-      <c r="P28" s="13" t="s">
-        <v>493</v>
-      </c>
-      <c r="Q28" s="13" t="s">
-        <v>494</v>
-      </c>
-      <c r="R28" s="13" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="29" spans="2:18" ht="64.5" thickBot="1">
+        <v>584</v>
+      </c>
+      <c r="N28" s="12"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+    </row>
+    <row r="29" spans="2:18" ht="15.75" thickBot="1">
       <c r="B29" t="s">
-        <v>366</v>
+        <v>573</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>369</v>
+        <v>568</v>
       </c>
       <c r="E29" t="s">
         <v>355</v>
       </c>
-      <c r="F29" t="s">
-        <v>551</v>
-      </c>
       <c r="G29" t="s">
         <v>356</v>
       </c>
@@ -3112,42 +3171,29 @@
         <v>359</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="K29" t="s">
-        <v>361</v>
-      </c>
-      <c r="N29" s="12" t="s">
-        <v>496</v>
-      </c>
-      <c r="O29" s="13">
-        <v>670</v>
-      </c>
-      <c r="P29" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="Q29" s="13" t="s">
-        <v>498</v>
-      </c>
-      <c r="R29" s="13" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="30" spans="2:18" ht="26.25" thickBot="1">
+        <v>584</v>
+      </c>
+      <c r="N29" s="12"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="13"/>
+    </row>
+    <row r="30" spans="2:18" ht="45.75" thickBot="1">
       <c r="B30" t="s">
-        <v>367</v>
+        <v>574</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>369</v>
+        <v>568</v>
       </c>
       <c r="E30" t="s">
         <v>355</v>
       </c>
-      <c r="F30" t="s">
-        <v>551</v>
+      <c r="F30" s="2" t="s">
+        <v>576</v>
       </c>
       <c r="G30" t="s">
         <v>356</v>
@@ -3159,41 +3205,27 @@
         <v>359</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="K30" t="s">
-        <v>361</v>
-      </c>
-      <c r="N30" s="12" t="s">
-        <v>499</v>
-      </c>
-      <c r="O30" s="13">
-        <v>534</v>
-      </c>
-      <c r="P30" s="13" t="s">
-        <v>500</v>
-      </c>
-      <c r="Q30" s="13" t="s">
-        <v>501</v>
-      </c>
+        <v>584</v>
+      </c>
+      <c r="N30" s="12"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
       <c r="R30" s="13"/>
     </row>
-    <row r="31" spans="2:18" ht="39" thickBot="1">
+    <row r="31" spans="2:18" ht="15.75" thickBot="1">
       <c r="B31" t="s">
-        <v>368</v>
+        <v>575</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>369</v>
+        <v>568</v>
       </c>
       <c r="E31" t="s">
         <v>355</v>
       </c>
-      <c r="F31" t="s">
-        <v>551</v>
-      </c>
       <c r="G31" t="s">
         <v>356</v>
       </c>
@@ -3204,30 +3236,17 @@
         <v>359</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="K31" t="s">
-        <v>361</v>
-      </c>
-      <c r="N31" s="12" t="s">
-        <v>502</v>
-      </c>
-      <c r="O31" s="13">
-        <v>780</v>
-      </c>
-      <c r="P31" s="13" t="s">
-        <v>503</v>
-      </c>
-      <c r="Q31" s="13" t="s">
-        <v>504</v>
-      </c>
-      <c r="R31" s="13" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="32" spans="2:18" ht="39" thickBot="1">
+        <v>584</v>
+      </c>
+      <c r="N31" s="12"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+    </row>
+    <row r="32" spans="2:18" ht="26.25" thickBot="1">
       <c r="B32" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3257,24 +3276,24 @@
         <v>361</v>
       </c>
       <c r="N32" s="12" t="s">
-        <v>506</v>
+        <v>477</v>
       </c>
       <c r="O32" s="13">
-        <v>796</v>
+        <v>630</v>
       </c>
       <c r="P32" s="13" t="s">
-        <v>507</v>
+        <v>478</v>
       </c>
       <c r="Q32" s="13" t="s">
-        <v>508</v>
+        <v>479</v>
       </c>
       <c r="R32" s="13" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="33" spans="2:18" ht="51.75" thickBot="1">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" ht="39" thickBot="1">
       <c r="B33" t="s">
-        <v>26</v>
+        <v>363</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -3304,187 +3323,427 @@
         <v>361</v>
       </c>
       <c r="N33" s="12" t="s">
-        <v>510</v>
+        <v>481</v>
       </c>
       <c r="O33" s="13">
-        <v>850</v>
+        <v>652</v>
       </c>
       <c r="P33" s="13" t="s">
-        <v>437</v>
+        <v>482</v>
       </c>
       <c r="Q33" s="13" t="s">
-        <v>511</v>
-      </c>
-      <c r="R33" s="13" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="34" spans="2:18" ht="25.5">
-      <c r="N34" s="10" t="s">
-        <v>513</v>
-      </c>
-      <c r="O34" s="11">
-        <v>13</v>
-      </c>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="11"/>
-    </row>
-    <row r="35" spans="2:18" ht="15.75" thickBot="1">
+        <v>483</v>
+      </c>
+      <c r="R33" s="13"/>
+    </row>
+    <row r="34" spans="2:18" ht="26.25" thickBot="1">
+      <c r="B34" t="s">
+        <v>364</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>369</v>
+      </c>
+      <c r="E34" t="s">
+        <v>355</v>
+      </c>
+      <c r="F34" t="s">
+        <v>551</v>
+      </c>
+      <c r="G34" t="s">
+        <v>356</v>
+      </c>
+      <c r="H34" t="s">
+        <v>358</v>
+      </c>
+      <c r="I34" t="s">
+        <v>359</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="K34" t="s">
+        <v>361</v>
+      </c>
+      <c r="N34" s="12" t="s">
+        <v>484</v>
+      </c>
+      <c r="O34" s="13">
+        <v>659</v>
+      </c>
+      <c r="P34" s="13" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q34" s="13" t="s">
+        <v>486</v>
+      </c>
+      <c r="R34" s="13" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" ht="26.25" thickBot="1">
+      <c r="B35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>369</v>
+      </c>
+      <c r="E35" t="s">
+        <v>355</v>
+      </c>
+      <c r="F35" t="s">
+        <v>551</v>
+      </c>
+      <c r="G35" t="s">
+        <v>356</v>
+      </c>
+      <c r="H35" t="s">
+        <v>358</v>
+      </c>
+      <c r="I35" t="s">
+        <v>359</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="K35" t="s">
+        <v>361</v>
+      </c>
       <c r="N35" s="12" t="s">
-        <v>514</v>
+        <v>488</v>
       </c>
       <c r="O35" s="13">
-        <v>84</v>
+        <v>662</v>
       </c>
       <c r="P35" s="13" t="s">
-        <v>515</v>
+        <v>489</v>
       </c>
       <c r="Q35" s="13" t="s">
-        <v>516</v>
+        <v>490</v>
       </c>
       <c r="R35" s="13" t="s">
-        <v>517</v>
+        <v>491</v>
       </c>
     </row>
     <row r="36" spans="2:18" ht="26.25" thickBot="1">
       <c r="B36" t="s">
-        <v>20</v>
+        <v>365</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>369</v>
+      </c>
+      <c r="E36" t="s">
+        <v>355</v>
+      </c>
+      <c r="F36" t="s">
+        <v>551</v>
+      </c>
+      <c r="G36" t="s">
+        <v>356</v>
+      </c>
+      <c r="H36" t="s">
+        <v>358</v>
+      </c>
+      <c r="I36" t="s">
+        <v>359</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="K36" t="s">
+        <v>361</v>
       </c>
       <c r="N36" s="12" t="s">
-        <v>518</v>
+        <v>492</v>
       </c>
       <c r="O36" s="13">
-        <v>188</v>
+        <v>663</v>
       </c>
       <c r="P36" s="13" t="s">
-        <v>519</v>
+        <v>493</v>
       </c>
       <c r="Q36" s="13" t="s">
-        <v>520</v>
+        <v>494</v>
       </c>
       <c r="R36" s="13" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="37" spans="2:18" ht="26.25" thickBot="1">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" ht="64.5" thickBot="1">
       <c r="B37" t="s">
-        <v>21</v>
+        <v>366</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>369</v>
+      </c>
+      <c r="E37" t="s">
+        <v>355</v>
+      </c>
+      <c r="F37" t="s">
+        <v>551</v>
+      </c>
+      <c r="G37" t="s">
+        <v>356</v>
+      </c>
+      <c r="H37" t="s">
+        <v>358</v>
+      </c>
+      <c r="I37" t="s">
+        <v>359</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="K37" t="s">
+        <v>361</v>
       </c>
       <c r="N37" s="12" t="s">
-        <v>522</v>
+        <v>496</v>
       </c>
       <c r="O37" s="13">
-        <v>222</v>
+        <v>670</v>
       </c>
       <c r="P37" s="13" t="s">
-        <v>523</v>
+        <v>497</v>
       </c>
       <c r="Q37" s="13" t="s">
-        <v>524</v>
+        <v>498</v>
       </c>
       <c r="R37" s="13" t="s">
-        <v>525</v>
+        <v>497</v>
       </c>
     </row>
     <row r="38" spans="2:18" ht="26.25" thickBot="1">
       <c r="B38" t="s">
-        <v>22</v>
+        <v>367</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>369</v>
+      </c>
+      <c r="E38" t="s">
+        <v>355</v>
+      </c>
+      <c r="F38" t="s">
+        <v>551</v>
+      </c>
+      <c r="G38" t="s">
+        <v>356</v>
+      </c>
+      <c r="H38" t="s">
+        <v>358</v>
+      </c>
+      <c r="I38" t="s">
+        <v>359</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="K38" t="s">
+        <v>361</v>
       </c>
       <c r="N38" s="12" t="s">
-        <v>526</v>
+        <v>499</v>
       </c>
       <c r="O38" s="13">
-        <v>320</v>
+        <v>534</v>
       </c>
       <c r="P38" s="13" t="s">
-        <v>527</v>
+        <v>500</v>
       </c>
       <c r="Q38" s="13" t="s">
-        <v>528</v>
-      </c>
-      <c r="R38" s="13" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="39" spans="2:18" ht="15.75" thickBot="1">
+        <v>501</v>
+      </c>
+      <c r="R38" s="13"/>
+    </row>
+    <row r="39" spans="2:18" ht="39" thickBot="1">
       <c r="B39" t="s">
-        <v>23</v>
+        <v>368</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>369</v>
+      </c>
+      <c r="E39" t="s">
+        <v>355</v>
+      </c>
+      <c r="F39" t="s">
+        <v>551</v>
+      </c>
+      <c r="G39" t="s">
+        <v>356</v>
+      </c>
+      <c r="H39" t="s">
+        <v>358</v>
+      </c>
+      <c r="I39" t="s">
+        <v>359</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="K39" t="s">
+        <v>361</v>
       </c>
       <c r="N39" s="12" t="s">
-        <v>529</v>
+        <v>502</v>
       </c>
       <c r="O39" s="13">
-        <v>340</v>
+        <v>780</v>
       </c>
       <c r="P39" s="13" t="s">
-        <v>530</v>
+        <v>503</v>
       </c>
       <c r="Q39" s="13" t="s">
-        <v>531</v>
+        <v>504</v>
       </c>
       <c r="R39" s="13" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="40" spans="2:18" ht="15.75" thickBot="1">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="40" spans="2:18" ht="39" thickBot="1">
       <c r="B40" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
-      <c r="N40" s="12"/>
-      <c r="O40" s="13"/>
-      <c r="P40" s="13"/>
-      <c r="Q40" s="13"/>
-      <c r="R40" s="13"/>
-    </row>
-    <row r="41" spans="2:18" ht="15.75" thickBot="1">
+      <c r="D40" t="s">
+        <v>369</v>
+      </c>
+      <c r="E40" t="s">
+        <v>355</v>
+      </c>
+      <c r="F40" t="s">
+        <v>551</v>
+      </c>
+      <c r="G40" t="s">
+        <v>356</v>
+      </c>
+      <c r="H40" t="s">
+        <v>358</v>
+      </c>
+      <c r="I40" t="s">
+        <v>359</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="K40" t="s">
+        <v>361</v>
+      </c>
+      <c r="N40" s="12" t="s">
+        <v>506</v>
+      </c>
+      <c r="O40" s="13">
+        <v>796</v>
+      </c>
+      <c r="P40" s="13" t="s">
+        <v>507</v>
+      </c>
+      <c r="Q40" s="13" t="s">
+        <v>508</v>
+      </c>
+      <c r="R40" s="13" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="41" spans="2:18" ht="51.75" thickBot="1">
       <c r="B41" t="s">
-        <v>363</v>
+        <v>26</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
-      <c r="N41" s="12"/>
-      <c r="O41" s="13"/>
-      <c r="P41" s="13"/>
-      <c r="Q41" s="13"/>
-      <c r="R41" s="13"/>
-    </row>
-    <row r="42" spans="2:18" ht="15.75" thickBot="1">
-      <c r="B42" t="s">
-        <v>364</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="N42" s="12"/>
-      <c r="O42" s="13"/>
-      <c r="P42" s="13"/>
-      <c r="Q42" s="13"/>
-      <c r="R42" s="13"/>
+      <c r="D41" t="s">
+        <v>369</v>
+      </c>
+      <c r="E41" t="s">
+        <v>355</v>
+      </c>
+      <c r="F41" t="s">
+        <v>551</v>
+      </c>
+      <c r="G41" t="s">
+        <v>356</v>
+      </c>
+      <c r="H41" t="s">
+        <v>358</v>
+      </c>
+      <c r="I41" t="s">
+        <v>359</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="K41" t="s">
+        <v>361</v>
+      </c>
+      <c r="N41" s="12" t="s">
+        <v>510</v>
+      </c>
+      <c r="O41" s="13">
+        <v>850</v>
+      </c>
+      <c r="P41" s="13" t="s">
+        <v>437</v>
+      </c>
+      <c r="Q41" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="R41" s="13" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="42" spans="2:18" ht="25.5">
+      <c r="N42" s="10" t="s">
+        <v>513</v>
+      </c>
+      <c r="O42" s="11">
+        <v>13</v>
+      </c>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
     </row>
     <row r="43" spans="2:18" ht="15.75" thickBot="1">
       <c r="B43" t="s">
-        <v>19</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="N43" s="12"/>
-      <c r="O43" s="13"/>
-      <c r="P43" s="13"/>
-      <c r="Q43" s="13"/>
-      <c r="R43" s="13"/>
+        <v>20</v>
+      </c>
+      <c r="N43" s="12" t="s">
+        <v>514</v>
+      </c>
+      <c r="O43" s="13">
+        <v>84</v>
+      </c>
+      <c r="P43" s="13" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q43" s="13" t="s">
+        <v>516</v>
+      </c>
+      <c r="R43" s="13" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="44" spans="2:18" ht="15.75" thickBot="1">
       <c r="B44" t="s">
-        <v>365</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="N44" s="12"/>
       <c r="O44" s="13"/>
@@ -3494,739 +3753,1175 @@
     </row>
     <row r="45" spans="2:18" ht="15.75" thickBot="1">
       <c r="B45" t="s">
-        <v>366</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="N45" s="12" t="s">
-        <v>533</v>
-      </c>
-      <c r="O45" s="13">
-        <v>484</v>
-      </c>
-      <c r="P45" s="13" t="s">
-        <v>534</v>
-      </c>
-      <c r="Q45" s="13" t="s">
-        <v>535</v>
-      </c>
-      <c r="R45" s="13" t="s">
-        <v>534</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="N45" s="12"/>
+      <c r="O45" s="13"/>
+      <c r="P45" s="13"/>
+      <c r="Q45" s="13"/>
+      <c r="R45" s="13"/>
     </row>
     <row r="46" spans="2:18" ht="15.75" thickBot="1">
       <c r="B46" t="s">
-        <v>367</v>
-      </c>
-      <c r="C46">
+        <v>23</v>
+      </c>
+      <c r="N46" s="12"/>
+      <c r="O46" s="13"/>
+      <c r="P46" s="13"/>
+      <c r="Q46" s="13"/>
+      <c r="R46" s="13"/>
+    </row>
+    <row r="47" spans="2:18" ht="105.75" thickBot="1">
+      <c r="B47" t="s">
+        <v>577</v>
+      </c>
+      <c r="D47" t="s">
+        <v>568</v>
+      </c>
+      <c r="E47" t="s">
+        <v>355</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="G47" t="s">
+        <v>356</v>
+      </c>
+      <c r="H47" t="s">
+        <v>358</v>
+      </c>
+      <c r="I47" t="s">
+        <v>359</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="N47" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="O47" s="13">
+        <v>188</v>
+      </c>
+      <c r="P47" s="13" t="s">
+        <v>519</v>
+      </c>
+      <c r="Q47" s="13" t="s">
+        <v>520</v>
+      </c>
+      <c r="R47" s="13" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="48" spans="2:18" ht="26.25" thickBot="1">
+      <c r="B48" t="s">
+        <v>578</v>
+      </c>
+      <c r="D48" t="s">
+        <v>568</v>
+      </c>
+      <c r="E48" t="s">
+        <v>355</v>
+      </c>
+      <c r="G48" t="s">
+        <v>356</v>
+      </c>
+      <c r="H48" t="s">
+        <v>358</v>
+      </c>
+      <c r="I48" t="s">
+        <v>359</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="N48" s="12" t="s">
+        <v>522</v>
+      </c>
+      <c r="O48" s="13">
+        <v>222</v>
+      </c>
+      <c r="P48" s="13" t="s">
+        <v>523</v>
+      </c>
+      <c r="Q48" s="13" t="s">
+        <v>524</v>
+      </c>
+      <c r="R48" s="13" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="49" spans="2:18" ht="105.75" thickBot="1">
+      <c r="B49" t="s">
+        <v>579</v>
+      </c>
+      <c r="D49" t="s">
+        <v>568</v>
+      </c>
+      <c r="E49" t="s">
+        <v>355</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="G49" t="s">
+        <v>356</v>
+      </c>
+      <c r="H49" t="s">
+        <v>358</v>
+      </c>
+      <c r="I49" t="s">
+        <v>359</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="N49" s="12" t="s">
+        <v>526</v>
+      </c>
+      <c r="O49" s="13">
+        <v>320</v>
+      </c>
+      <c r="P49" s="13" t="s">
+        <v>527</v>
+      </c>
+      <c r="Q49" s="13" t="s">
+        <v>528</v>
+      </c>
+      <c r="R49" s="13" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="50" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B50" t="s">
+        <v>580</v>
+      </c>
+      <c r="D50" t="s">
+        <v>568</v>
+      </c>
+      <c r="E50" t="s">
+        <v>355</v>
+      </c>
+      <c r="G50" t="s">
+        <v>356</v>
+      </c>
+      <c r="H50" t="s">
+        <v>358</v>
+      </c>
+      <c r="I50" t="s">
+        <v>359</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="N50" s="12" t="s">
+        <v>529</v>
+      </c>
+      <c r="O50" s="13">
+        <v>340</v>
+      </c>
+      <c r="P50" s="13" t="s">
+        <v>530</v>
+      </c>
+      <c r="Q50" s="13" t="s">
+        <v>531</v>
+      </c>
+      <c r="R50" s="13" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="51" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B51" t="s">
+        <v>553</v>
+      </c>
+      <c r="C51">
         <v>1</v>
       </c>
-      <c r="N46" s="12" t="s">
+      <c r="D51" t="s">
+        <v>562</v>
+      </c>
+      <c r="E51" t="s">
+        <v>355</v>
+      </c>
+      <c r="F51" t="s">
+        <v>535</v>
+      </c>
+      <c r="G51" t="s">
+        <v>356</v>
+      </c>
+      <c r="H51" t="s">
+        <v>358</v>
+      </c>
+      <c r="I51" t="s">
+        <v>359</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="K51" t="s">
+        <v>361</v>
+      </c>
+      <c r="N51" s="12"/>
+      <c r="O51" s="13"/>
+      <c r="P51" s="13"/>
+      <c r="Q51" s="13"/>
+      <c r="R51" s="13"/>
+    </row>
+    <row r="52" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B52" t="s">
+        <v>554</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>562</v>
+      </c>
+      <c r="E52" t="s">
+        <v>355</v>
+      </c>
+      <c r="F52" t="s">
+        <v>535</v>
+      </c>
+      <c r="G52" t="s">
+        <v>356</v>
+      </c>
+      <c r="H52" t="s">
+        <v>358</v>
+      </c>
+      <c r="I52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="K52" t="s">
+        <v>361</v>
+      </c>
+      <c r="N52" s="12"/>
+      <c r="O52" s="13"/>
+      <c r="P52" s="13"/>
+      <c r="Q52" s="13"/>
+      <c r="R52" s="13"/>
+    </row>
+    <row r="53" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B53" t="s">
+        <v>555</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>562</v>
+      </c>
+      <c r="E53" t="s">
+        <v>355</v>
+      </c>
+      <c r="F53" t="s">
+        <v>535</v>
+      </c>
+      <c r="G53" t="s">
+        <v>356</v>
+      </c>
+      <c r="H53" t="s">
+        <v>358</v>
+      </c>
+      <c r="I53" t="s">
+        <v>359</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="K53" t="s">
+        <v>361</v>
+      </c>
+      <c r="N53" s="12"/>
+      <c r="O53" s="13"/>
+      <c r="P53" s="13"/>
+      <c r="Q53" s="13"/>
+      <c r="R53" s="13"/>
+    </row>
+    <row r="54" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B54" t="s">
+        <v>556</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
+        <v>562</v>
+      </c>
+      <c r="E54" t="s">
+        <v>355</v>
+      </c>
+      <c r="F54" t="s">
+        <v>535</v>
+      </c>
+      <c r="G54" t="s">
+        <v>356</v>
+      </c>
+      <c r="H54" t="s">
+        <v>358</v>
+      </c>
+      <c r="I54" t="s">
+        <v>359</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="K54" t="s">
+        <v>361</v>
+      </c>
+      <c r="N54" s="12"/>
+      <c r="O54" s="13"/>
+      <c r="P54" s="13"/>
+      <c r="Q54" s="13"/>
+      <c r="R54" s="13"/>
+    </row>
+    <row r="55" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B55" t="s">
+        <v>557</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>562</v>
+      </c>
+      <c r="E55" t="s">
+        <v>355</v>
+      </c>
+      <c r="F55" t="s">
+        <v>535</v>
+      </c>
+      <c r="G55" t="s">
+        <v>356</v>
+      </c>
+      <c r="H55" t="s">
+        <v>358</v>
+      </c>
+      <c r="I55" t="s">
+        <v>359</v>
+      </c>
+      <c r="J55" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="K55" t="s">
+        <v>361</v>
+      </c>
+      <c r="N55" s="12"/>
+      <c r="O55" s="13"/>
+      <c r="P55" s="13"/>
+      <c r="Q55" s="13"/>
+      <c r="R55" s="13"/>
+    </row>
+    <row r="56" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B56" t="s">
+        <v>558</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>562</v>
+      </c>
+      <c r="E56" t="s">
+        <v>355</v>
+      </c>
+      <c r="F56" t="s">
+        <v>535</v>
+      </c>
+      <c r="G56" t="s">
+        <v>356</v>
+      </c>
+      <c r="H56" t="s">
+        <v>358</v>
+      </c>
+      <c r="I56" t="s">
+        <v>359</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="K56" t="s">
+        <v>361</v>
+      </c>
+      <c r="N56" s="12" t="s">
+        <v>533</v>
+      </c>
+      <c r="O56" s="13">
+        <v>484</v>
+      </c>
+      <c r="P56" s="13" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q56" s="13" t="s">
+        <v>535</v>
+      </c>
+      <c r="R56" s="13" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="57" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B57" t="s">
+        <v>559</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>562</v>
+      </c>
+      <c r="E57" t="s">
+        <v>355</v>
+      </c>
+      <c r="F57" t="s">
+        <v>535</v>
+      </c>
+      <c r="G57" t="s">
+        <v>356</v>
+      </c>
+      <c r="H57" t="s">
+        <v>358</v>
+      </c>
+      <c r="I57" t="s">
+        <v>359</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="K57" t="s">
+        <v>361</v>
+      </c>
+      <c r="N57" s="12" t="s">
         <v>536</v>
       </c>
-      <c r="O46" s="13">
+      <c r="O57" s="13">
         <v>558</v>
       </c>
-      <c r="P46" s="13" t="s">
+      <c r="P57" s="13" t="s">
         <v>537</v>
       </c>
-      <c r="Q46" s="13" t="s">
+      <c r="Q57" s="13" t="s">
         <v>538</v>
       </c>
-      <c r="R46" s="13" t="s">
+      <c r="R57" s="13" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="47" spans="2:18" ht="15.75" thickBot="1">
-      <c r="B47" t="s">
-        <v>368</v>
-      </c>
-      <c r="C47">
+    <row r="58" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B58" t="s">
+        <v>560</v>
+      </c>
+      <c r="C58">
         <v>1</v>
       </c>
-      <c r="N47" s="12" t="s">
+      <c r="D58" t="s">
+        <v>562</v>
+      </c>
+      <c r="E58" t="s">
+        <v>355</v>
+      </c>
+      <c r="F58" t="s">
+        <v>535</v>
+      </c>
+      <c r="G58" t="s">
+        <v>356</v>
+      </c>
+      <c r="H58" t="s">
+        <v>358</v>
+      </c>
+      <c r="I58" t="s">
+        <v>359</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="K58" t="s">
+        <v>361</v>
+      </c>
+      <c r="N58" s="12" t="s">
         <v>540</v>
       </c>
-      <c r="O47" s="13">
+      <c r="O58" s="13">
         <v>591</v>
       </c>
-      <c r="P47" s="13" t="s">
+      <c r="P58" s="13" t="s">
         <v>541</v>
       </c>
-      <c r="Q47" s="13" t="s">
+      <c r="Q58" s="13" t="s">
         <v>542</v>
       </c>
-      <c r="R47" s="13" t="s">
+      <c r="R58" s="13" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="48" spans="2:18" ht="25.5">
-      <c r="B48" t="s">
+    <row r="59" spans="2:18" ht="25.5">
+      <c r="B59" t="s">
         <v>25</v>
       </c>
-      <c r="C48">
+      <c r="C59">
         <v>1</v>
       </c>
-      <c r="N48" s="10" t="s">
+      <c r="D59" t="s">
+        <v>562</v>
+      </c>
+      <c r="E59" t="s">
+        <v>355</v>
+      </c>
+      <c r="F59" t="s">
+        <v>535</v>
+      </c>
+      <c r="G59" t="s">
+        <v>356</v>
+      </c>
+      <c r="H59" t="s">
+        <v>358</v>
+      </c>
+      <c r="I59" t="s">
+        <v>359</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="K59" t="s">
+        <v>361</v>
+      </c>
+      <c r="N59" s="10" t="s">
         <v>544</v>
       </c>
-      <c r="O48" s="11">
+      <c r="O59" s="11">
         <v>5</v>
       </c>
-      <c r="P48" s="11"/>
-      <c r="Q48" s="11"/>
-      <c r="R48" s="11"/>
-    </row>
-    <row r="49" spans="1:18" ht="15.75" thickBot="1">
-      <c r="B49" t="s">
-        <v>26</v>
-      </c>
-      <c r="C49">
+      <c r="P59" s="11"/>
+      <c r="Q59" s="11"/>
+      <c r="R59" s="11"/>
+    </row>
+    <row r="60" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B60" t="s">
+        <v>561</v>
+      </c>
+      <c r="C60">
         <v>1</v>
       </c>
-      <c r="N49" s="12" t="s">
+      <c r="D60" t="s">
+        <v>562</v>
+      </c>
+      <c r="E60" t="s">
+        <v>355</v>
+      </c>
+      <c r="F60" t="s">
+        <v>535</v>
+      </c>
+      <c r="G60" t="s">
+        <v>356</v>
+      </c>
+      <c r="H60" t="s">
+        <v>358</v>
+      </c>
+      <c r="I60" t="s">
+        <v>359</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="K60" t="s">
+        <v>361</v>
+      </c>
+      <c r="N60" s="12" t="s">
         <v>370</v>
       </c>
-      <c r="O49" s="13">
+      <c r="O60" s="13">
         <v>32</v>
       </c>
-      <c r="P49" s="13" t="s">
+      <c r="P60" s="13" t="s">
         <v>371</v>
       </c>
-      <c r="Q49" s="13" t="s">
+      <c r="Q60" s="13" t="s">
         <v>372</v>
       </c>
-      <c r="R49" s="13" t="s">
+      <c r="R60" s="13" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="51.75" thickBot="1">
-      <c r="N50" s="12" t="s">
+    <row r="61" spans="2:18" ht="51.75" thickBot="1">
+      <c r="N61" s="12" t="s">
         <v>545</v>
       </c>
-      <c r="O50" s="13">
+      <c r="O61" s="13">
         <v>68</v>
       </c>
-      <c r="P50" s="13" t="s">
+      <c r="P61" s="13" t="s">
         <v>373</v>
       </c>
-      <c r="Q50" s="13" t="s">
+      <c r="Q61" s="13" t="s">
         <v>374</v>
       </c>
-      <c r="R50" s="13" t="s">
+      <c r="R61" s="13" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="15.75" thickBot="1">
-      <c r="B51" t="s">
+    <row r="62" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B62" t="s">
         <v>340</v>
       </c>
-      <c r="N51" s="12" t="s">
+      <c r="N62" s="12" t="s">
         <v>375</v>
       </c>
-      <c r="O51" s="13">
+      <c r="O62" s="13">
         <v>76</v>
       </c>
-      <c r="P51" s="13" t="s">
+      <c r="P62" s="13" t="s">
         <v>376</v>
       </c>
-      <c r="Q51" s="13" t="s">
+      <c r="Q62" s="13" t="s">
         <v>377</v>
       </c>
-      <c r="R51" s="13" t="s">
+      <c r="R62" s="13" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="15.75" thickBot="1">
-      <c r="B52" t="s">
+    <row r="63" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B63" t="s">
         <v>341</v>
       </c>
-      <c r="N52" s="12" t="s">
+      <c r="N63" s="12" t="s">
         <v>378</v>
       </c>
-      <c r="O52" s="13">
+      <c r="O63" s="13">
         <v>152</v>
       </c>
-      <c r="P52" s="13" t="s">
+      <c r="P63" s="13" t="s">
         <v>379</v>
       </c>
-      <c r="Q52" s="13" t="s">
+      <c r="Q63" s="13" t="s">
         <v>380</v>
       </c>
-      <c r="R52" s="13" t="s">
+      <c r="R63" s="13" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="15.75" thickBot="1">
-      <c r="B53" t="s">
+    <row r="64" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B64" t="s">
         <v>342</v>
       </c>
-      <c r="N53" s="12" t="s">
+      <c r="N64" s="12" t="s">
         <v>381</v>
       </c>
-      <c r="O53" s="13">
+      <c r="O64" s="13">
         <v>170</v>
       </c>
-      <c r="P53" s="13" t="s">
+      <c r="P64" s="13" t="s">
         <v>382</v>
       </c>
-      <c r="Q53" s="13" t="s">
+      <c r="Q64" s="13" t="s">
         <v>383</v>
       </c>
-      <c r="R53" s="13" t="s">
+      <c r="R64" s="13" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="15.75" thickBot="1">
-      <c r="B54" t="s">
+    <row r="65" spans="1:18" ht="15.75" thickBot="1">
+      <c r="B65" t="s">
         <v>343</v>
       </c>
-      <c r="N54" s="12" t="s">
+      <c r="N65" s="12" t="s">
         <v>384</v>
       </c>
-      <c r="O54" s="13">
+      <c r="O65" s="13">
         <v>218</v>
       </c>
-      <c r="P54" s="13" t="s">
+      <c r="P65" s="13" t="s">
         <v>385</v>
       </c>
-      <c r="Q54" s="13" t="s">
+      <c r="Q65" s="13" t="s">
         <v>386</v>
       </c>
-      <c r="R54" s="13" t="s">
+      <c r="R65" s="13" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="55" spans="1:18" ht="51.75" thickBot="1">
-      <c r="B55" t="s">
+    <row r="66" spans="1:18" ht="15.75" thickBot="1">
+      <c r="B66" t="s">
+        <v>564</v>
+      </c>
+      <c r="N66" s="12"/>
+      <c r="O66" s="13"/>
+      <c r="P66" s="13"/>
+      <c r="Q66" s="13"/>
+      <c r="R66" s="13"/>
+    </row>
+    <row r="67" spans="1:18" ht="15.75" thickBot="1">
+      <c r="B67" t="s">
+        <v>566</v>
+      </c>
+      <c r="N67" s="12"/>
+      <c r="O67" s="13"/>
+      <c r="P67" s="13"/>
+      <c r="Q67" s="13"/>
+      <c r="R67" s="13"/>
+    </row>
+    <row r="68" spans="1:18" ht="15.75" thickBot="1">
+      <c r="B68" t="s">
+        <v>565</v>
+      </c>
+      <c r="N68" s="12"/>
+      <c r="O68" s="13"/>
+      <c r="P68" s="13"/>
+      <c r="Q68" s="13"/>
+      <c r="R68" s="13"/>
+    </row>
+    <row r="69" spans="1:18" ht="15.75" thickBot="1">
+      <c r="B69" t="s">
+        <v>567</v>
+      </c>
+      <c r="N69" s="12"/>
+      <c r="O69" s="13"/>
+      <c r="P69" s="13"/>
+      <c r="Q69" s="13"/>
+      <c r="R69" s="13"/>
+    </row>
+    <row r="70" spans="1:18" ht="51.75" thickBot="1">
+      <c r="B70" t="s">
         <v>344</v>
       </c>
-      <c r="N55" s="12" t="s">
+      <c r="N70" s="12" t="s">
         <v>547</v>
       </c>
-      <c r="O55" s="13">
+      <c r="O70" s="13">
         <v>238</v>
       </c>
-      <c r="P55" s="13" t="s">
+      <c r="P70" s="13" t="s">
         <v>387</v>
       </c>
-      <c r="Q55" s="13" t="s">
+      <c r="Q70" s="13" t="s">
         <v>388</v>
       </c>
-      <c r="R55" s="13" t="s">
+      <c r="R70" s="13" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="26.25" thickBot="1">
-      <c r="B56" t="s">
+    <row r="71" spans="1:18" ht="26.25" thickBot="1">
+      <c r="B71" t="s">
         <v>24</v>
       </c>
-      <c r="N56" s="12" t="s">
+      <c r="N71" s="12" t="s">
         <v>389</v>
       </c>
-      <c r="O56" s="13">
+      <c r="O71" s="13">
         <v>254</v>
       </c>
-      <c r="P56" s="13" t="s">
+      <c r="P71" s="13" t="s">
         <v>390</v>
       </c>
-      <c r="Q56" s="13" t="s">
+      <c r="Q71" s="13" t="s">
         <v>391</v>
       </c>
-      <c r="R56" s="13" t="s">
+      <c r="R71" s="13" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="15.75" thickBot="1">
-      <c r="B57" t="s">
+    <row r="72" spans="1:18" ht="15.75" thickBot="1">
+      <c r="B72" t="s">
         <v>345</v>
       </c>
-      <c r="N57" s="12" t="s">
+      <c r="N72" s="12" t="s">
         <v>393</v>
       </c>
-      <c r="O57" s="13">
+      <c r="O72" s="13">
         <v>328</v>
       </c>
-      <c r="P57" s="13" t="s">
+      <c r="P72" s="13" t="s">
         <v>392</v>
       </c>
-      <c r="Q57" s="13" t="s">
+      <c r="Q72" s="13" t="s">
         <v>394</v>
       </c>
-      <c r="R57" s="13" t="s">
+      <c r="R72" s="13" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="15.75" thickBot="1">
-      <c r="B58" t="s">
+    <row r="73" spans="1:18" ht="15.75" thickBot="1">
+      <c r="B73" t="s">
         <v>346</v>
       </c>
-      <c r="N58" s="12" t="s">
+      <c r="N73" s="12" t="s">
         <v>395</v>
       </c>
-      <c r="O58" s="13">
+      <c r="O73" s="13">
         <v>600</v>
       </c>
-      <c r="P58" s="13" t="s">
+      <c r="P73" s="13" t="s">
         <v>396</v>
       </c>
-      <c r="Q58" s="13" t="s">
+      <c r="Q73" s="13" t="s">
         <v>397</v>
       </c>
-      <c r="R58" s="13" t="s">
+      <c r="R73" s="13" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="15.75" thickBot="1">
-      <c r="B59" t="s">
+    <row r="74" spans="1:18" ht="15.75" thickBot="1">
+      <c r="B74" t="s">
         <v>347</v>
       </c>
-      <c r="N59" s="12" t="s">
+      <c r="N74" s="12" t="s">
         <v>398</v>
       </c>
-      <c r="O59" s="13">
+      <c r="O74" s="13">
         <v>604</v>
       </c>
-      <c r="P59" s="13" t="s">
+      <c r="P74" s="13" t="s">
         <v>399</v>
       </c>
-      <c r="Q59" s="13" t="s">
+      <c r="Q74" s="13" t="s">
         <v>400</v>
       </c>
-      <c r="R59" s="13" t="s">
+      <c r="R74" s="13" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="15.75" thickBot="1">
-      <c r="N60" s="12" t="s">
+    <row r="75" spans="1:18" ht="15.75" thickBot="1">
+      <c r="N75" s="12" t="s">
         <v>401</v>
       </c>
-      <c r="O60" s="13">
+      <c r="O75" s="13">
         <v>740</v>
       </c>
-      <c r="P60" s="13" t="s">
+      <c r="P75" s="13" t="s">
         <v>402</v>
       </c>
-      <c r="Q60" s="13" t="s">
+      <c r="Q75" s="13" t="s">
         <v>403</v>
       </c>
-      <c r="R60" s="13" t="s">
+      <c r="R75" s="13" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="61" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A61" t="s">
+    <row r="76" spans="1:18" ht="15.75" thickBot="1">
+      <c r="A76" t="s">
         <v>31</v>
       </c>
-      <c r="N61" s="12" t="s">
+      <c r="N76" s="12" t="s">
         <v>404</v>
       </c>
-      <c r="O61" s="13">
+      <c r="O76" s="13">
         <v>858</v>
       </c>
-      <c r="P61" s="13" t="s">
+      <c r="P76" s="13" t="s">
         <v>405</v>
       </c>
-      <c r="Q61" s="13" t="s">
+      <c r="Q76" s="13" t="s">
         <v>406</v>
       </c>
-      <c r="R61" s="13" t="s">
+      <c r="R76" s="13" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="64.5" thickBot="1">
-      <c r="B62" t="s">
+    <row r="77" spans="1:18" ht="64.5" thickBot="1">
+      <c r="B77" t="s">
         <v>34</v>
       </c>
-      <c r="N62" s="12" t="s">
+      <c r="N77" s="12" t="s">
         <v>550</v>
       </c>
-      <c r="O62" s="13">
+      <c r="O77" s="13">
         <v>862</v>
       </c>
-      <c r="P62" s="13" t="s">
+      <c r="P77" s="13" t="s">
         <v>407</v>
       </c>
-      <c r="Q62" s="13" t="s">
+      <c r="Q77" s="13" t="s">
         <v>408</v>
       </c>
-      <c r="R62" s="13" t="s">
+      <c r="R77" s="13" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="63" spans="1:18">
-      <c r="B63" t="s">
+    <row r="78" spans="1:18">
+      <c r="B78" t="s">
         <v>35</v>
       </c>
-      <c r="N63" s="1"/>
-    </row>
-    <row r="64" spans="1:18">
-      <c r="B64" t="s">
+      <c r="N78" s="1"/>
+    </row>
+    <row r="79" spans="1:18">
+      <c r="B79" t="s">
         <v>32</v>
       </c>
-      <c r="N64" s="1"/>
-    </row>
-    <row r="65" spans="1:14">
-      <c r="B65" t="s">
+      <c r="N79" s="1"/>
+    </row>
+    <row r="80" spans="1:18">
+      <c r="B80" t="s">
         <v>33</v>
-      </c>
-      <c r="N65" s="1"/>
-    </row>
-    <row r="66" spans="1:14">
-      <c r="B66" t="s">
-        <v>36</v>
-      </c>
-      <c r="N66" s="1"/>
-    </row>
-    <row r="67" spans="1:14">
-      <c r="B67" t="s">
-        <v>37</v>
-      </c>
-      <c r="N67" s="1"/>
-    </row>
-    <row r="68" spans="1:14">
-      <c r="B68" t="s">
-        <v>38</v>
-      </c>
-      <c r="N68" s="1"/>
-    </row>
-    <row r="69" spans="1:14">
-      <c r="B69" t="s">
-        <v>58</v>
-      </c>
-      <c r="N69" s="1"/>
-    </row>
-    <row r="70" spans="1:14">
-      <c r="B70" t="s">
-        <v>59</v>
-      </c>
-      <c r="N70" s="1"/>
-    </row>
-    <row r="71" spans="1:14">
-      <c r="B71" t="s">
-        <v>39</v>
-      </c>
-      <c r="N71" s="1"/>
-    </row>
-    <row r="72" spans="1:14">
-      <c r="B72" t="s">
-        <v>40</v>
-      </c>
-      <c r="N72" s="1"/>
-    </row>
-    <row r="73" spans="1:14">
-      <c r="B73" t="s">
-        <v>41</v>
-      </c>
-      <c r="N73" s="1"/>
-    </row>
-    <row r="74" spans="1:14">
-      <c r="B74" t="s">
-        <v>42</v>
-      </c>
-      <c r="N74" s="1"/>
-    </row>
-    <row r="75" spans="1:14">
-      <c r="N75" s="1"/>
-    </row>
-    <row r="76" spans="1:14">
-      <c r="A76" t="s">
-        <v>43</v>
-      </c>
-      <c r="N76" s="1"/>
-    </row>
-    <row r="77" spans="1:14">
-      <c r="B77" t="s">
-        <v>44</v>
-      </c>
-      <c r="N77" s="1"/>
-    </row>
-    <row r="78" spans="1:14">
-      <c r="B78" t="s">
-        <v>45</v>
-      </c>
-      <c r="N78" s="1"/>
-    </row>
-    <row r="79" spans="1:14">
-      <c r="B79" t="s">
-        <v>46</v>
-      </c>
-      <c r="N79" s="1"/>
-    </row>
-    <row r="80" spans="1:14">
-      <c r="B80" t="s">
-        <v>47</v>
       </c>
       <c r="N80" s="1"/>
     </row>
     <row r="81" spans="1:14">
       <c r="B81" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="N81" s="1"/>
     </row>
     <row r="82" spans="1:14">
       <c r="B82" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="N82" s="1"/>
     </row>
     <row r="83" spans="1:14">
       <c r="B83" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="N83" s="1"/>
     </row>
     <row r="84" spans="1:14">
       <c r="B84" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="N84" s="1"/>
     </row>
     <row r="85" spans="1:14">
       <c r="B85" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="N85" s="1"/>
     </row>
     <row r="86" spans="1:14">
       <c r="B86" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="N86" s="1"/>
     </row>
     <row r="87" spans="1:14">
       <c r="B87" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="N87" s="1"/>
     </row>
     <row r="88" spans="1:14">
       <c r="B88" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="N88" s="1"/>
     </row>
     <row r="89" spans="1:14">
       <c r="B89" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="N89" s="1"/>
     </row>
     <row r="90" spans="1:14">
-      <c r="B90" t="s">
-        <v>65</v>
-      </c>
       <c r="N90" s="1"/>
     </row>
     <row r="91" spans="1:14">
-      <c r="B91" t="s">
-        <v>66</v>
+      <c r="A91" t="s">
+        <v>43</v>
       </c>
       <c r="N91" s="1"/>
     </row>
     <row r="92" spans="1:14">
       <c r="B92" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="N92" s="1"/>
     </row>
     <row r="93" spans="1:14">
+      <c r="B93" t="s">
+        <v>45</v>
+      </c>
       <c r="N93" s="1"/>
     </row>
     <row r="94" spans="1:14">
-      <c r="A94" t="s">
-        <v>56</v>
+      <c r="B94" t="s">
+        <v>46</v>
       </c>
       <c r="N94" s="1"/>
     </row>
     <row r="95" spans="1:14">
       <c r="B95" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="N95" s="1"/>
     </row>
     <row r="96" spans="1:14">
       <c r="B96" t="s">
+        <v>48</v>
+      </c>
+      <c r="N96" s="1"/>
+    </row>
+    <row r="97" spans="1:14">
+      <c r="B97" t="s">
+        <v>49</v>
+      </c>
+      <c r="N97" s="1"/>
+    </row>
+    <row r="98" spans="1:14">
+      <c r="B98" t="s">
+        <v>50</v>
+      </c>
+      <c r="N98" s="1"/>
+    </row>
+    <row r="99" spans="1:14">
+      <c r="B99" t="s">
+        <v>51</v>
+      </c>
+      <c r="N99" s="1"/>
+    </row>
+    <row r="100" spans="1:14">
+      <c r="B100" t="s">
+        <v>52</v>
+      </c>
+      <c r="N100" s="1"/>
+    </row>
+    <row r="101" spans="1:14">
+      <c r="B101" t="s">
+        <v>53</v>
+      </c>
+      <c r="N101" s="1"/>
+    </row>
+    <row r="102" spans="1:14">
+      <c r="B102" t="s">
+        <v>54</v>
+      </c>
+      <c r="N102" s="1"/>
+    </row>
+    <row r="103" spans="1:14">
+      <c r="B103" t="s">
+        <v>55</v>
+      </c>
+      <c r="N103" s="1"/>
+    </row>
+    <row r="104" spans="1:14">
+      <c r="B104" t="s">
+        <v>64</v>
+      </c>
+      <c r="N104" s="1"/>
+    </row>
+    <row r="105" spans="1:14">
+      <c r="B105" t="s">
+        <v>65</v>
+      </c>
+      <c r="N105" s="1"/>
+    </row>
+    <row r="106" spans="1:14">
+      <c r="B106" t="s">
+        <v>66</v>
+      </c>
+      <c r="N106" s="1"/>
+    </row>
+    <row r="107" spans="1:14">
+      <c r="B107" t="s">
+        <v>67</v>
+      </c>
+      <c r="N107" s="1"/>
+    </row>
+    <row r="108" spans="1:14">
+      <c r="N108" s="1"/>
+    </row>
+    <row r="109" spans="1:14">
+      <c r="A109" t="s">
+        <v>56</v>
+      </c>
+      <c r="N109" s="1"/>
+    </row>
+    <row r="110" spans="1:14">
+      <c r="B110" t="s">
+        <v>62</v>
+      </c>
+      <c r="N110" s="1"/>
+    </row>
+    <row r="111" spans="1:14">
+      <c r="B111" t="s">
         <v>57</v>
       </c>
-      <c r="N96" s="1"/>
-    </row>
-    <row r="97" spans="2:14">
-      <c r="B97" t="s">
+      <c r="N111" s="1"/>
+    </row>
+    <row r="112" spans="1:14">
+      <c r="B112" t="s">
         <v>60</v>
       </c>
-      <c r="N97" s="1"/>
-    </row>
-    <row r="98" spans="2:14">
-      <c r="B98" t="s">
+      <c r="N112" s="1"/>
+    </row>
+    <row r="113" spans="1:14">
+      <c r="B113" t="s">
         <v>61</v>
-      </c>
-      <c r="N98" s="1"/>
-    </row>
-    <row r="99" spans="2:14">
-      <c r="B99" t="s">
-        <v>63</v>
-      </c>
-      <c r="N99" s="1"/>
-    </row>
-    <row r="100" spans="2:14">
-      <c r="B100" t="s">
-        <v>68</v>
-      </c>
-      <c r="N100" s="1"/>
-    </row>
-    <row r="101" spans="2:14">
-      <c r="B101" t="s">
-        <v>69</v>
-      </c>
-      <c r="N101" s="1"/>
-    </row>
-    <row r="102" spans="2:14">
-      <c r="B102" t="s">
-        <v>70</v>
-      </c>
-      <c r="N102" s="1"/>
-    </row>
-    <row r="103" spans="2:14">
-      <c r="B103" t="s">
-        <v>71</v>
-      </c>
-      <c r="N103" s="1"/>
-    </row>
-    <row r="104" spans="2:14">
-      <c r="B104" t="s">
-        <v>72</v>
-      </c>
-      <c r="N104" s="1"/>
-    </row>
-    <row r="105" spans="2:14">
-      <c r="B105" t="s">
-        <v>73</v>
-      </c>
-      <c r="N105" s="1"/>
-    </row>
-    <row r="106" spans="2:14">
-      <c r="B106" t="s">
-        <v>74</v>
-      </c>
-      <c r="N106" s="1"/>
-    </row>
-    <row r="107" spans="2:14">
-      <c r="B107" t="s">
-        <v>75</v>
-      </c>
-      <c r="N107" s="1"/>
-    </row>
-    <row r="108" spans="2:14">
-      <c r="B108" t="s">
-        <v>76</v>
-      </c>
-      <c r="N108" s="1"/>
-    </row>
-    <row r="109" spans="2:14">
-      <c r="B109" t="s">
-        <v>77</v>
-      </c>
-      <c r="N109" s="1"/>
-    </row>
-    <row r="110" spans="2:14">
-      <c r="B110" t="s">
-        <v>78</v>
-      </c>
-      <c r="N110" s="1"/>
-    </row>
-    <row r="111" spans="2:14">
-      <c r="B111" t="s">
-        <v>79</v>
-      </c>
-      <c r="N111" s="1"/>
-    </row>
-    <row r="112" spans="2:14">
-      <c r="N112" s="1"/>
-    </row>
-    <row r="113" spans="1:14">
-      <c r="A113" t="s">
-        <v>80</v>
       </c>
       <c r="N113" s="1"/>
     </row>
     <row r="114" spans="1:14">
       <c r="B114" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="N114" s="1"/>
     </row>
     <row r="115" spans="1:14">
       <c r="B115" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="N115" s="1"/>
     </row>
     <row r="116" spans="1:14">
       <c r="B116" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="N116" s="1"/>
     </row>
     <row r="117" spans="1:14">
       <c r="B117" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="N117" s="1"/>
     </row>
     <row r="118" spans="1:14">
       <c r="B118" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="N118" s="1"/>
     </row>
     <row r="119" spans="1:14">
       <c r="B119" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="N119" s="1"/>
     </row>
     <row r="120" spans="1:14">
       <c r="B120" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="N120" s="1"/>
     </row>
     <row r="121" spans="1:14">
       <c r="B121" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="N121" s="1"/>
     </row>
     <row r="122" spans="1:14">
       <c r="B122" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="N122" s="1"/>
     </row>
     <row r="123" spans="1:14">
       <c r="B123" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="N123" s="1"/>
     </row>
     <row r="124" spans="1:14">
       <c r="B124" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="N124" s="1"/>
     </row>
     <row r="125" spans="1:14">
       <c r="B125" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="N125" s="1"/>
     </row>
     <row r="126" spans="1:14">
       <c r="B126" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="N126" s="1"/>
     </row>
@@ -4234,54 +4929,96 @@
       <c r="N127" s="1"/>
     </row>
     <row r="128" spans="1:14">
+      <c r="A128" t="s">
+        <v>80</v>
+      </c>
       <c r="N128" s="1"/>
     </row>
-    <row r="129" spans="14:14">
+    <row r="129" spans="2:14">
+      <c r="B129" t="s">
+        <v>53</v>
+      </c>
       <c r="N129" s="1"/>
     </row>
-    <row r="130" spans="14:14">
+    <row r="130" spans="2:14">
+      <c r="B130" t="s">
+        <v>81</v>
+      </c>
       <c r="N130" s="1"/>
     </row>
-    <row r="131" spans="14:14">
+    <row r="131" spans="2:14">
+      <c r="B131" t="s">
+        <v>82</v>
+      </c>
       <c r="N131" s="1"/>
     </row>
-    <row r="132" spans="14:14">
+    <row r="132" spans="2:14">
+      <c r="B132" t="s">
+        <v>83</v>
+      </c>
       <c r="N132" s="1"/>
     </row>
-    <row r="133" spans="14:14">
+    <row r="133" spans="2:14">
+      <c r="B133" t="s">
+        <v>84</v>
+      </c>
       <c r="N133" s="1"/>
     </row>
-    <row r="134" spans="14:14">
+    <row r="134" spans="2:14">
+      <c r="B134" t="s">
+        <v>85</v>
+      </c>
       <c r="N134" s="1"/>
     </row>
-    <row r="135" spans="14:14">
+    <row r="135" spans="2:14">
+      <c r="B135" t="s">
+        <v>86</v>
+      </c>
       <c r="N135" s="1"/>
     </row>
-    <row r="136" spans="14:14">
+    <row r="136" spans="2:14">
+      <c r="B136" t="s">
+        <v>87</v>
+      </c>
       <c r="N136" s="1"/>
     </row>
-    <row r="137" spans="14:14">
+    <row r="137" spans="2:14">
+      <c r="B137" t="s">
+        <v>88</v>
+      </c>
       <c r="N137" s="1"/>
     </row>
-    <row r="138" spans="14:14">
+    <row r="138" spans="2:14">
+      <c r="B138" t="s">
+        <v>89</v>
+      </c>
       <c r="N138" s="1"/>
     </row>
-    <row r="139" spans="14:14">
+    <row r="139" spans="2:14">
+      <c r="B139" t="s">
+        <v>90</v>
+      </c>
       <c r="N139" s="1"/>
     </row>
-    <row r="140" spans="14:14">
+    <row r="140" spans="2:14">
+      <c r="B140" t="s">
+        <v>91</v>
+      </c>
       <c r="N140" s="1"/>
     </row>
-    <row r="141" spans="14:14">
+    <row r="141" spans="2:14">
+      <c r="B141" t="s">
+        <v>92</v>
+      </c>
       <c r="N141" s="1"/>
     </row>
-    <row r="142" spans="14:14">
+    <row r="142" spans="2:14">
       <c r="N142" s="1"/>
     </row>
-    <row r="143" spans="14:14">
+    <row r="143" spans="2:14">
       <c r="N143" s="1"/>
     </row>
-    <row r="144" spans="14:14">
+    <row r="144" spans="2:14">
       <c r="N144" s="1"/>
     </row>
     <row r="145" spans="14:14">
@@ -4665,24 +5402,87 @@
     <row r="271" spans="14:14">
       <c r="N271" s="1"/>
     </row>
+    <row r="272" spans="14:14">
+      <c r="N272" s="1"/>
+    </row>
+    <row r="273" spans="14:14">
+      <c r="N273" s="1"/>
+    </row>
+    <row r="274" spans="14:14">
+      <c r="N274" s="1"/>
+    </row>
+    <row r="275" spans="14:14">
+      <c r="N275" s="1"/>
+    </row>
+    <row r="276" spans="14:14">
+      <c r="N276" s="1"/>
+    </row>
+    <row r="277" spans="14:14">
+      <c r="N277" s="1"/>
+    </row>
+    <row r="278" spans="14:14">
+      <c r="N278" s="1"/>
+    </row>
+    <row r="279" spans="14:14">
+      <c r="N279" s="1"/>
+    </row>
+    <row r="280" spans="14:14">
+      <c r="N280" s="1"/>
+    </row>
+    <row r="281" spans="14:14">
+      <c r="N281" s="1"/>
+    </row>
+    <row r="282" spans="14:14">
+      <c r="N282" s="1"/>
+    </row>
+    <row r="283" spans="14:14">
+      <c r="N283" s="1"/>
+    </row>
+    <row r="284" spans="14:14">
+      <c r="N284" s="1"/>
+    </row>
+    <row r="285" spans="14:14">
+      <c r="N285" s="1"/>
+    </row>
+    <row r="286" spans="14:14">
+      <c r="N286" s="1"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J9" r:id="rId1"/>
-    <hyperlink ref="J10:J17" r:id="rId2" display="operaciones_gobierno_central_all_years_all_countries_cepalstat.xlsx"/>
-    <hyperlink ref="J18" r:id="rId3"/>
-    <hyperlink ref="J24" r:id="rId4"/>
-    <hyperlink ref="J25" r:id="rId5"/>
-    <hyperlink ref="J26" r:id="rId6"/>
-    <hyperlink ref="J27" r:id="rId7"/>
-    <hyperlink ref="J28" r:id="rId8"/>
-    <hyperlink ref="J29" r:id="rId9"/>
-    <hyperlink ref="J30" r:id="rId10"/>
-    <hyperlink ref="J31" r:id="rId11"/>
-    <hyperlink ref="J32" r:id="rId12"/>
-    <hyperlink ref="J33" r:id="rId13"/>
+    <hyperlink ref="J13" r:id="rId1"/>
+    <hyperlink ref="J14:J21" r:id="rId2" display="operaciones_gobierno_central_all_years_all_countries_cepalstat.xlsx"/>
+    <hyperlink ref="J22" r:id="rId3"/>
+    <hyperlink ref="J32" r:id="rId4"/>
+    <hyperlink ref="J33" r:id="rId5"/>
+    <hyperlink ref="J34" r:id="rId6"/>
+    <hyperlink ref="J35" r:id="rId7"/>
+    <hyperlink ref="J36" r:id="rId8"/>
+    <hyperlink ref="J37" r:id="rId9"/>
+    <hyperlink ref="J38" r:id="rId10"/>
+    <hyperlink ref="J39" r:id="rId11"/>
+    <hyperlink ref="J40" r:id="rId12"/>
+    <hyperlink ref="J41" r:id="rId13"/>
+    <hyperlink ref="J51" r:id="rId14"/>
+    <hyperlink ref="J52" r:id="rId15"/>
+    <hyperlink ref="J53" r:id="rId16"/>
+    <hyperlink ref="J54" r:id="rId17"/>
+    <hyperlink ref="J55" r:id="rId18"/>
+    <hyperlink ref="J56" r:id="rId19"/>
+    <hyperlink ref="J57" r:id="rId20"/>
+    <hyperlink ref="J58" r:id="rId21"/>
+    <hyperlink ref="J59" r:id="rId22"/>
+    <hyperlink ref="J60" r:id="rId23"/>
+    <hyperlink ref="J47" r:id="rId24"/>
+    <hyperlink ref="J48:J50" r:id="rId25" display="financiamiento_spnf_central_all_years_all_alc_cepalstat.xlsx"/>
+    <hyperlink ref="J28" r:id="rId26"/>
+    <hyperlink ref="J29" r:id="rId27"/>
+    <hyperlink ref="J30" r:id="rId28"/>
+    <hyperlink ref="J31" r:id="rId29"/>
+    <hyperlink ref="J9" r:id="rId30"/>
+    <hyperlink ref="J10:J12" r:id="rId31" display="financiamiento_gobierno_central_all_years_all_alc_cepalstat.xlsx"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
 

</xml_diff>